<commit_message>
Completed lab 3.4.2, 3.6.1
</commit_message>
<xml_diff>
--- a/Physics/3.6.1/3.6.1.xlsx
+++ b/Physics/3.6.1/3.6.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIPT-MIPS\Labs\Physics\3.6.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CB5EB0-8B47-4E07-928B-5798CF95CAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504BE6EF-ED34-4D48-AD52-7A0C6260D45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{9BA1F08E-355E-484E-A3A3-D771CBF81F12}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>\tau, мкс</t>
   </si>
@@ -91,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -195,20 +195,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -526,7 +583,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J2" sqref="J2:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,6 +591,7 @@
     <col min="1" max="1" width="20.1796875" customWidth="1"/>
     <col min="4" max="4" width="13.7265625" customWidth="1"/>
     <col min="7" max="7" width="11.81640625" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
@@ -543,23 +601,26 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="9" t="s">
         <v>8</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -569,157 +630,236 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
+      <c r="A2" s="2">
         <v>32.5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>25</v>
       </c>
-      <c r="D2">
+      <c r="C2">
+        <f>1/B2</f>
+        <v>0.04</v>
+      </c>
+      <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="10">
         <v>1</v>
       </c>
       <c r="G2">
         <v>2.83</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>2.4</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="10">
         <v>0</v>
       </c>
+      <c r="J2" s="10">
+        <f>(H2-I2)/(H2+I2)</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="10">
+        <f>1/G2</f>
+        <v>0.35335689045936397</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>17.5</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>50</v>
       </c>
-      <c r="D3">
+      <c r="C3">
+        <f t="shared" ref="C3:C9" si="0">1/B3</f>
+        <v>0.02</v>
+      </c>
+      <c r="D3" s="5">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="11">
         <v>3</v>
       </c>
       <c r="G3">
         <v>3.2</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="5">
         <v>2</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="11">
         <v>0.4</v>
       </c>
+      <c r="J3" s="11">
+        <f t="shared" ref="J3:J7" si="1">(H3-I3)/(H3+I3)</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="K3" s="11">
+        <f t="shared" ref="K3:K6" si="2">1/G3</f>
+        <v>0.3125</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>12</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <v>75</v>
       </c>
-      <c r="D4">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="D4" s="5">
         <v>4</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="11">
         <v>4</v>
       </c>
       <c r="G4">
         <v>4.25</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="5">
         <v>1.8</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="11">
         <v>0.6</v>
       </c>
+      <c r="J4" s="11">
+        <f t="shared" si="1"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="K4" s="11">
+        <f t="shared" si="2"/>
+        <v>0.23529411764705882</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>8</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>100</v>
       </c>
-      <c r="D5">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="5">
         <v>6</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="11">
         <v>6</v>
       </c>
       <c r="G5">
         <v>6</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="5">
         <v>1.6</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="11">
         <v>0.8</v>
       </c>
+      <c r="J5" s="11">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>7</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="5">
         <v>125</v>
       </c>
-      <c r="D6">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D6" s="5">
         <v>7</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="11">
         <v>7</v>
       </c>
       <c r="G6">
         <v>11</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="5">
         <v>1.4</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="11">
         <v>1</v>
       </c>
+      <c r="J6" s="11">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="K6" s="11">
+        <f t="shared" si="2"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="5">
         <v>150</v>
       </c>
-      <c r="D7">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666671E-3</v>
+      </c>
+      <c r="D7" s="7">
         <v>8</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="12">
         <v>8</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="7">
         <v>1.2</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="12">
         <v>1.2</v>
       </c>
+      <c r="J7" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="5">
         <v>175</v>
       </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>5.7142857142857143E-3</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>4</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="7">
         <v>200</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>